<commit_message>
reporte de actividades de 12 diciembre semana
</commit_message>
<xml_diff>
--- a/Horas Extra/2022/12.Dec2022.xlsx
+++ b/Horas Extra/2022/12.Dec2022.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Velandia Juan\Desktop\horasExtra\Horas Extra\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo.velandia\Desktop\horasExtra\Horas Extra\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991BC024-F109-4533-AC38-F7E807728FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="REPORTE HORAS EXTRAS" sheetId="7" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'REPORTE HORAS EXTRAS'!$A$1:$K$54</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -165,13 +164,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-240A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1187,10 +1186,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1205,87 +1286,6 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1307,13 +1307,12 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 6" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1348,7 +1347,7 @@
         <xdr:cNvPr id="4" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1408,7 +1407,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1483,23 +1482,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1535,23 +1517,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1727,128 +1692,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14" style="122" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="7" width="20.33203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="109" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="31.44140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="40.5546875" style="12" customWidth="1"/>
+    <col min="6" max="7" width="20.36328125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="20.36328125" style="109" customWidth="1"/>
+    <col min="9" max="9" width="20.36328125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="31.453125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="21.36328125" customWidth="1"/>
+    <col min="12" max="12" width="40.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129"/>
-      <c r="B1" s="130"/>
-      <c r="C1" s="146" t="s">
+    <row r="1" spans="1:25" ht="11.25" customHeight="1">
+      <c r="A1" s="124"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="140" t="s">
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="141"/>
-    </row>
-    <row r="2" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="131"/>
-      <c r="B2" s="132"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="141"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="141"/>
-    </row>
-    <row r="3" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="131"/>
-      <c r="B3" s="132"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="149"/>
-      <c r="H3" s="149"/>
-      <c r="I3" s="149"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="140" t="s">
+      <c r="L1" s="136"/>
+    </row>
+    <row r="2" spans="1:25" ht="11.25" customHeight="1">
+      <c r="A2" s="126"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="135"/>
+      <c r="L2" s="136"/>
+    </row>
+    <row r="3" spans="1:25" ht="11.25" customHeight="1">
+      <c r="A3" s="126"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="141"/>
+      <c r="L3" s="136"/>
       <c r="N3" s="22"/>
     </row>
-    <row r="4" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="131"/>
-      <c r="B4" s="132"/>
-      <c r="C4" s="138" t="s">
+    <row r="4" spans="1:25" ht="11.25" customHeight="1">
+      <c r="A4" s="126"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="142"/>
-      <c r="L4" s="143"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="138"/>
       <c r="N4" s="22"/>
     </row>
-    <row r="5" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="131"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="138"/>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="144" t="s">
+    <row r="5" spans="1:25" ht="11.25" customHeight="1">
+      <c r="A5" s="126"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="139" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="145"/>
-    </row>
-    <row r="6" spans="1:25" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="133"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="140"/>
-      <c r="L6" s="141"/>
-    </row>
-    <row r="7" spans="1:25" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="140"/>
+    </row>
+    <row r="6" spans="1:25" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A6" s="128"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="136"/>
+    </row>
+    <row r="7" spans="1:25" ht="6" customHeight="1" thickBot="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
@@ -1862,7 +1827,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>1</v>
       </c>
@@ -1888,7 +1853,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="11.25" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="58"/>
       <c r="C9" s="58"/>
@@ -1905,7 +1870,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:25" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="6.75" customHeight="1" thickBot="1">
       <c r="A10" s="10"/>
       <c r="B10" s="63"/>
       <c r="C10" s="63"/>
@@ -1919,55 +1884,55 @@
       <c r="K10" s="66"/>
       <c r="L10" s="65"/>
     </row>
-    <row r="11" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="135" t="s">
+    <row r="11" spans="1:25" ht="12.75" customHeight="1">
+      <c r="A11" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="123"/>
-      <c r="D11" s="152" t="s">
+      <c r="C11" s="147"/>
+      <c r="D11" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="150" t="s">
+      <c r="F11" s="145" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="150" t="s">
+      <c r="G11" s="145" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="152" t="s">
+      <c r="H11" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="123" t="s">
+      <c r="I11" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="123" t="s">
+      <c r="J11" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="150" t="s">
+      <c r="K11" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="154" t="s">
+      <c r="L11" s="151" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="136"/>
-      <c r="B12" s="124"/>
-      <c r="C12" s="124"/>
-      <c r="D12" s="153"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="151"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="153"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="151"/>
-      <c r="L12" s="155"/>
+    <row r="12" spans="1:25" ht="12.75" customHeight="1">
+      <c r="A12" s="131"/>
+      <c r="B12" s="148"/>
+      <c r="C12" s="148"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="148"/>
+      <c r="J12" s="148"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="152"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1982,23 +1947,23 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="137"/>
+    <row r="13" spans="1:25" ht="22.5" customHeight="1">
+      <c r="A13" s="132"/>
       <c r="B13" s="51" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="153"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="151"/>
-      <c r="H13" s="153"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="151"/>
-      <c r="L13" s="155"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="146"/>
+      <c r="H13" s="150"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="148"/>
+      <c r="K13" s="146"/>
+      <c r="L13" s="152"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -2013,7 +1978,7 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="79.25" customHeight="1">
       <c r="A14" s="88">
         <v>44903</v>
       </c>
@@ -2024,7 +1989,9 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D14" s="94"/>
-      <c r="E14" s="89"/>
+      <c r="E14" s="100">
+        <v>6</v>
+      </c>
       <c r="F14" s="90"/>
       <c r="G14" s="91"/>
       <c r="H14" s="100"/>
@@ -2050,10 +2017,10 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="63.65" customHeight="1">
       <c r="A15" s="88"/>
-      <c r="B15" s="163"/>
-      <c r="C15" s="163"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
       <c r="D15" s="94"/>
       <c r="E15" s="89"/>
       <c r="F15" s="90"/>
@@ -2077,7 +2044,7 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="42.65" customHeight="1">
       <c r="A16" s="88"/>
       <c r="B16" s="93"/>
       <c r="C16" s="93"/>
@@ -2104,7 +2071,7 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="56" customHeight="1">
       <c r="A17" s="88"/>
       <c r="B17" s="93"/>
       <c r="C17" s="93"/>
@@ -2131,7 +2098,7 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="47.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="47.75" customHeight="1">
       <c r="A18" s="87"/>
       <c r="B18" s="92"/>
       <c r="C18" s="93"/>
@@ -2158,7 +2125,7 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" ht="63.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="63.5" customHeight="1">
       <c r="A19" s="87"/>
       <c r="B19" s="92"/>
       <c r="C19" s="93"/>
@@ -2185,7 +2152,7 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="58.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="59" customHeight="1">
       <c r="A20" s="21"/>
       <c r="B20" s="77"/>
       <c r="C20" s="78"/>
@@ -2212,7 +2179,7 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" ht="46.5" customHeight="1">
       <c r="A21" s="21"/>
       <c r="B21" s="40"/>
       <c r="C21" s="41"/>
@@ -2239,7 +2206,7 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="37.25" customHeight="1">
       <c r="A22" s="21"/>
       <c r="B22" s="40"/>
       <c r="C22" s="41"/>
@@ -2266,7 +2233,7 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="42" customHeight="1">
       <c r="A23" s="42"/>
       <c r="B23" s="40"/>
       <c r="C23" s="41"/>
@@ -2293,7 +2260,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" ht="43.25" customHeight="1">
       <c r="A24" s="42"/>
       <c r="B24" s="40"/>
       <c r="C24" s="41"/>
@@ -2320,7 +2287,7 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="45" customHeight="1">
       <c r="A25" s="45"/>
       <c r="B25" s="40"/>
       <c r="C25" s="41"/>
@@ -2347,7 +2314,7 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A26" s="45"/>
       <c r="B26" s="40"/>
       <c r="C26" s="41"/>
@@ -2374,7 +2341,7 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A27" s="45"/>
       <c r="B27" s="40"/>
       <c r="C27" s="41"/>
@@ -2401,7 +2368,7 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
     </row>
-    <row r="28" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A28" s="45"/>
       <c r="B28" s="40"/>
       <c r="C28" s="41"/>
@@ -2428,7 +2395,7 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A29" s="45"/>
       <c r="B29" s="40"/>
       <c r="C29" s="41"/>
@@ -2455,7 +2422,7 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A30" s="43"/>
       <c r="B30" s="40"/>
       <c r="C30" s="41"/>
@@ -2482,7 +2449,7 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A31" s="43"/>
       <c r="B31" s="40"/>
       <c r="C31" s="41"/>
@@ -2509,7 +2476,7 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A32" s="43"/>
       <c r="B32" s="40"/>
       <c r="C32" s="41"/>
@@ -2536,7 +2503,7 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A33" s="43"/>
       <c r="B33" s="40"/>
       <c r="C33" s="41"/>
@@ -2563,7 +2530,7 @@
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
     </row>
-    <row r="34" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A34" s="43"/>
       <c r="B34" s="40"/>
       <c r="C34" s="41"/>
@@ -2590,7 +2557,7 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
     </row>
-    <row r="35" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A35" s="43"/>
       <c r="B35" s="40"/>
       <c r="C35" s="41"/>
@@ -2617,7 +2584,7 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
     </row>
-    <row r="36" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A36" s="43"/>
       <c r="B36" s="40"/>
       <c r="C36" s="41"/>
@@ -2644,7 +2611,7 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A37" s="43"/>
       <c r="B37" s="40"/>
       <c r="C37" s="41"/>
@@ -2671,7 +2638,7 @@
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
     </row>
-    <row r="38" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A38" s="43"/>
       <c r="B38" s="40"/>
       <c r="C38" s="41"/>
@@ -2698,7 +2665,7 @@
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
     </row>
-    <row r="39" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A39" s="43"/>
       <c r="B39" s="40"/>
       <c r="C39" s="41"/>
@@ -2725,7 +2692,7 @@
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
     </row>
-    <row r="40" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A40" s="43"/>
       <c r="B40" s="40"/>
       <c r="C40" s="41"/>
@@ -2752,7 +2719,7 @@
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
     </row>
-    <row r="41" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A41" s="43"/>
       <c r="B41" s="40"/>
       <c r="C41" s="41"/>
@@ -2779,7 +2746,7 @@
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
     </row>
-    <row r="42" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A42" s="43"/>
       <c r="B42" s="40"/>
       <c r="C42" s="41"/>
@@ -2806,7 +2773,7 @@
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
     </row>
-    <row r="43" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" ht="20.149999999999999" customHeight="1">
       <c r="A43" s="43"/>
       <c r="B43" s="40"/>
       <c r="C43" s="41"/>
@@ -2833,7 +2800,7 @@
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
     </row>
-    <row r="44" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" ht="20.149999999999999" customHeight="1" thickBot="1">
       <c r="A44" s="35"/>
       <c r="B44" s="36"/>
       <c r="C44" s="36"/>
@@ -2860,12 +2827,12 @@
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
     </row>
-    <row r="45" spans="1:25" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="126" t="s">
+    <row r="45" spans="1:25" ht="20.149999999999999" customHeight="1" thickBot="1">
+      <c r="A45" s="154" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="127"/>
-      <c r="C45" s="128"/>
+      <c r="B45" s="155"/>
+      <c r="C45" s="156"/>
       <c r="D45" s="117">
         <f>SUM(D21:D44)</f>
         <v>0</v>
@@ -2904,18 +2871,18 @@
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
     </row>
-    <row r="47" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="24" customHeight="1">
       <c r="D47" s="118"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="125"/>
-      <c r="G47" s="125"/>
-      <c r="H47" s="125"/>
-      <c r="I47" s="125"/>
-      <c r="J47" s="125"/>
-      <c r="K47" s="125"/>
+      <c r="F47" s="153"/>
+      <c r="G47" s="153"/>
+      <c r="H47" s="153"/>
+      <c r="I47" s="153"/>
+      <c r="J47" s="153"/>
+      <c r="K47" s="153"/>
       <c r="L47" s="16"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="13">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -2929,13 +2896,13 @@
       <c r="K48" s="17"/>
       <c r="L48" s="14"/>
     </row>
-    <row r="49" spans="1:13" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="59.25" customHeight="1">
       <c r="A49" s="5"/>
-      <c r="B49" s="125"/>
-      <c r="C49" s="125"/>
+      <c r="B49" s="153"/>
+      <c r="C49" s="153"/>
       <c r="D49" s="120"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="125"/>
+      <c r="E49" s="153"/>
+      <c r="F49" s="153"/>
       <c r="G49" s="47"/>
       <c r="H49" s="107"/>
       <c r="I49" s="47"/>
@@ -2944,12 +2911,12 @@
       <c r="L49" s="14"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
+    <row r="50" spans="1:13" ht="13">
+      <c r="B50" s="153"/>
+      <c r="C50" s="153"/>
       <c r="D50" s="121"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="125"/>
+      <c r="E50" s="153"/>
+      <c r="F50" s="153"/>
       <c r="G50" s="47"/>
       <c r="H50" s="107"/>
       <c r="I50" s="47"/>
@@ -2958,7 +2925,7 @@
       <c r="L50" s="14"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="13">
       <c r="A51" s="5"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2973,7 +2940,7 @@
       <c r="L51" s="14"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="15.5">
       <c r="A52" s="5"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -2988,7 +2955,7 @@
       <c r="L52" s="14"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="15.5">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="121"/>
@@ -3002,7 +2969,7 @@
       <c r="L53" s="20"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="13">
       <c r="A54" s="5"/>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -3017,7 +2984,7 @@
       <c r="L54" s="14"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="13">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -3033,6 +3000,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="F47:K47"/>
     <mergeCell ref="A1:B6"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C4:J6"/>
@@ -3049,13 +3023,6 @@
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="F47:K47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3069,50 +3036,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="43.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.36328125" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="156" t="s">
+    <row r="1" spans="1:6" ht="13" thickBot="1"/>
+    <row r="2" spans="1:6" ht="15" thickBot="1">
+      <c r="A2" s="157" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="157"/>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="158"/>
-    </row>
-    <row r="3" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="159" t="s">
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="159"/>
+    </row>
+    <row r="3" spans="1:6" ht="14">
+      <c r="A3" s="160" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="162" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="162" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="67"/>
       <c r="E3" s="68"/>
       <c r="F3" s="68"/>
     </row>
-    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="160"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="162"/>
+    <row r="4" spans="1:6" ht="28">
+      <c r="A4" s="161"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
       <c r="D4" s="69" t="s">
         <v>28</v>
       </c>
@@ -3123,7 +3090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="20.25" customHeight="1" thickBot="1">
       <c r="A5" s="71" t="s">
         <v>31</v>
       </c>
@@ -3143,7 +3110,7 @@
         <v>42967</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="20.25" customHeight="1" thickBot="1">
       <c r="A6" s="71" t="s">
         <v>35</v>
       </c>
@@ -3163,7 +3130,7 @@
         <v>43132</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" thickBot="1">
       <c r="A7" s="71" t="s">
         <v>36</v>
       </c>

</xml_diff>